<commit_message>
Work on Traits and stats.xlsx
</commit_message>
<xml_diff>
--- a/Traits and stats.xlsx
+++ b/Traits and stats.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Professions" sheetId="1" r:id="rId1"/>
     <sheet name="Traits" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Religious</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Educator</t>
   </si>
   <si>
-    <t>Rural</t>
-  </si>
-  <si>
     <t>Law</t>
   </si>
   <si>
@@ -75,19 +72,46 @@
     <t>Diligence</t>
   </si>
   <si>
-    <t xml:space="preserve">Patience </t>
-  </si>
-  <si>
-    <t>Humble</t>
-  </si>
-  <si>
     <t>Kindness</t>
   </si>
   <si>
     <t>Greeds</t>
   </si>
   <si>
-    <t>Patience</t>
+    <t>Forgiveness</t>
+  </si>
+  <si>
+    <t>Humility</t>
+  </si>
+  <si>
+    <t>Farmer</t>
+  </si>
+  <si>
+    <t>Medical</t>
+  </si>
+  <si>
+    <t>Politics</t>
+  </si>
+  <si>
+    <t>Trades</t>
+  </si>
+  <si>
+    <t>Investigation</t>
+  </si>
+  <si>
+    <t>Recruitment</t>
+  </si>
+  <si>
+    <t>Abductions</t>
+  </si>
+  <si>
+    <t>Anti-Investigation</t>
+  </si>
+  <si>
+    <t>Anti-Recruitment</t>
+  </si>
+  <si>
+    <t>Anti-Abduction</t>
   </si>
 </sst>
 </file>
@@ -119,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -127,16 +151,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,36 +501,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -454,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,62 +636,71 @@
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>-10</v>
+      </c>
+      <c r="J2">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -532,11 +710,20 @@
       </c>
       <c r="D3">
         <v>5</v>
+      </c>
+      <c r="I3">
+        <v>-5</v>
+      </c>
+      <c r="J3">
+        <v>-10</v>
+      </c>
+      <c r="K3">
+        <v>-5</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -546,11 +733,20 @@
       </c>
       <c r="E4">
         <v>5</v>
+      </c>
+      <c r="J4">
+        <v>-5</v>
+      </c>
+      <c r="K4">
+        <v>-10</v>
+      </c>
+      <c r="L4">
+        <v>-5</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -560,11 +756,20 @@
       </c>
       <c r="F5">
         <v>5</v>
+      </c>
+      <c r="K5">
+        <v>-5</v>
+      </c>
+      <c r="L5">
+        <v>-10</v>
+      </c>
+      <c r="M5">
+        <v>-5</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -574,11 +779,20 @@
       </c>
       <c r="G6">
         <v>5</v>
+      </c>
+      <c r="L6">
+        <v>-5</v>
+      </c>
+      <c r="M6">
+        <v>-10</v>
+      </c>
+      <c r="N6">
+        <v>-5</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -588,11 +802,23 @@
       </c>
       <c r="H7">
         <v>5</v>
+      </c>
+      <c r="M7">
+        <v>-5</v>
+      </c>
+      <c r="N7">
+        <v>-10</v>
+      </c>
+      <c r="O7">
+        <v>-5</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -602,11 +828,23 @@
       </c>
       <c r="I8">
         <v>5</v>
+      </c>
+      <c r="N8">
+        <v>-5</v>
+      </c>
+      <c r="O8">
+        <v>-10</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>-10</v>
+      </c>
+      <c r="C9">
+        <v>-5</v>
       </c>
       <c r="H9">
         <v>5</v>
@@ -615,12 +853,24 @@
         <v>10</v>
       </c>
       <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="O9">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>-5</v>
+      </c>
+      <c r="C10">
+        <v>-10</v>
+      </c>
+      <c r="D10">
+        <v>-5</v>
       </c>
       <c r="I10">
         <v>5</v>
@@ -634,7 +884,16 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>-5</v>
+      </c>
+      <c r="D11">
+        <v>-10</v>
+      </c>
+      <c r="E11">
+        <v>-5</v>
       </c>
       <c r="J11">
         <v>5</v>
@@ -648,7 +907,16 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>-5</v>
+      </c>
+      <c r="E12">
+        <v>-10</v>
+      </c>
+      <c r="F12">
+        <v>-5</v>
       </c>
       <c r="K12">
         <v>5</v>
@@ -662,7 +930,16 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>-5</v>
+      </c>
+      <c r="F13">
+        <v>-10</v>
+      </c>
+      <c r="G13">
+        <v>-5</v>
       </c>
       <c r="L13">
         <v>5</v>
@@ -676,7 +953,16 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>-5</v>
+      </c>
+      <c r="G14">
+        <v>-10</v>
+      </c>
+      <c r="H14">
+        <v>-5</v>
       </c>
       <c r="M14">
         <v>5</v>
@@ -690,7 +976,19 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>-5</v>
+      </c>
+      <c r="G15">
+        <v>-5</v>
+      </c>
+      <c r="H15">
+        <v>-10</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
       </c>
       <c r="N15">
         <v>5</v>

</xml_diff>